<commit_message>
10.03.2023 - calculations complete
</commit_message>
<xml_diff>
--- a/resources/cwb-weapon-naming.xlsx
+++ b/resources/cwb-weapon-naming.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vasqu\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cvasquez\Desktop\cwb-calculator\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D7C2AC-5A25-499A-BDFC-CA1916A2409E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D512D674-66C2-4058-B091-6156B0BF909C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{67BC485C-6050-4687-9E5F-DD57FBD2EDC9}"/>
+    <workbookView xWindow="-24225" yWindow="2745" windowWidth="21600" windowHeight="11385" xr2:uid="{67BC485C-6050-4687-9E5F-DD57FBD2EDC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,14 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="109">
   <si>
     <t>Artillery</t>
   </si>
   <si>
-    <t>Firearms</t>
-  </si>
-  <si>
     <t>Smoothbore</t>
   </si>
   <si>
@@ -198,6 +195,174 @@
   </si>
   <si>
     <t xml:space="preserve">  Rifle Musket</t>
+  </si>
+  <si>
+    <t>Firearms Name</t>
+  </si>
+  <si>
+    <t>DB NAME</t>
+  </si>
+  <si>
+    <t>repeating</t>
+  </si>
+  <si>
+    <t>breechload</t>
+  </si>
+  <si>
+    <t>carbine</t>
+  </si>
+  <si>
+    <t>sb musket</t>
+  </si>
+  <si>
+    <t>pistol</t>
+  </si>
+  <si>
+    <t>rifle musket</t>
+  </si>
+  <si>
+    <t>shotgun</t>
+  </si>
+  <si>
+    <t>mixed arms</t>
+  </si>
+  <si>
+    <t>multiple arms</t>
+  </si>
+  <si>
+    <t>spencer carbine</t>
+  </si>
+  <si>
+    <t>sb 32pdr</t>
+  </si>
+  <si>
+    <t>sb 42pdr</t>
+  </si>
+  <si>
+    <t>sb napoleon</t>
+  </si>
+  <si>
+    <t>sb 12pdr wiard</t>
+  </si>
+  <si>
+    <t>sb 6pdr wiard</t>
+  </si>
+  <si>
+    <t>sb 6pdr</t>
+  </si>
+  <si>
+    <t>sb 24 pdr</t>
+  </si>
+  <si>
+    <t>rifled 32pdr</t>
+  </si>
+  <si>
+    <t>rifled 6pdr</t>
+  </si>
+  <si>
+    <t>rifled 3in</t>
+  </si>
+  <si>
+    <t>rifled 42pdr</t>
+  </si>
+  <si>
+    <t>rifled 18pdr</t>
+  </si>
+  <si>
+    <t>rifled 24pdr</t>
+  </si>
+  <si>
+    <t>rifled blakely</t>
+  </si>
+  <si>
+    <t>rifled brooke</t>
+  </si>
+  <si>
+    <t>rifled whitworth</t>
+  </si>
+  <si>
+    <t>rifled 4.5in</t>
+  </si>
+  <si>
+    <t>rifled 6.5in</t>
+  </si>
+  <si>
+    <t>rifled 3in naval</t>
+  </si>
+  <si>
+    <t>rifled 2.25in mtn</t>
+  </si>
+  <si>
+    <t>rifled 3.67in sawyer</t>
+  </si>
+  <si>
+    <t>col 10in</t>
+  </si>
+  <si>
+    <t>col 8in</t>
+  </si>
+  <si>
+    <t>siege 24pdr</t>
+  </si>
+  <si>
+    <t>ho 12pdr</t>
+  </si>
+  <si>
+    <t>ho 24pdr</t>
+  </si>
+  <si>
+    <t>ho 8in</t>
+  </si>
+  <si>
+    <t>ho 6.4in</t>
+  </si>
+  <si>
+    <t>ho 12pdr mountain</t>
+  </si>
+  <si>
+    <t>james 12pdr</t>
+  </si>
+  <si>
+    <t>james 6pdr</t>
+  </si>
+  <si>
+    <t>james 14pdr</t>
+  </si>
+  <si>
+    <t>parrott 20pdr</t>
+  </si>
+  <si>
+    <t>parrott 30pdr</t>
+  </si>
+  <si>
+    <t>parrott 10pdr</t>
+  </si>
+  <si>
+    <t>parrott 100pdr</t>
+  </si>
+  <si>
+    <t>parrott 200pdr</t>
+  </si>
+  <si>
+    <t>dahlgren 8in</t>
+  </si>
+  <si>
+    <t>dahlgren 9in</t>
+  </si>
+  <si>
+    <t>dahlgren 11in</t>
+  </si>
+  <si>
+    <t>mortar 13in</t>
+  </si>
+  <si>
+    <t>mortar 10in</t>
+  </si>
+  <si>
+    <t>mortar 24pdr coehorn</t>
+  </si>
+  <si>
+    <t>DBNAME</t>
   </si>
 </sst>
 </file>
@@ -579,31 +744,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6D50136-62AD-44F7-95AD-7A0D1833D35F}">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:T16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="124" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" customWidth="1"/>
+    <col min="13" max="13" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
@@ -611,229 +785,433 @@
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
-    </row>
-    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+    </row>
+    <row r="2" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="F2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="H2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="J2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="L2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="N2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="P2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="R2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="S2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="T2" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
+      <c r="H3" t="s">
+        <v>86</v>
+      </c>
+      <c r="I3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" t="s">
+        <v>88</v>
+      </c>
+      <c r="K3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" t="s">
+        <v>89</v>
+      </c>
+      <c r="M3" t="s">
+        <v>14</v>
+      </c>
+      <c r="N3" t="s">
+        <v>94</v>
+      </c>
+      <c r="O3" t="s">
+        <v>15</v>
+      </c>
+      <c r="P3" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R3" t="s">
+        <v>102</v>
+      </c>
+      <c r="S3" t="s">
+        <v>17</v>
+      </c>
+      <c r="T3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>87</v>
+      </c>
+      <c r="K4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4" t="s">
+        <v>90</v>
+      </c>
+      <c r="M4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N4" t="s">
+        <v>95</v>
+      </c>
+      <c r="O4" t="s">
+        <v>21</v>
+      </c>
+      <c r="P4" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>22</v>
+      </c>
+      <c r="R4" t="s">
+        <v>103</v>
+      </c>
+      <c r="S4" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
+      <c r="T4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" t="s">
+        <v>78</v>
+      </c>
+      <c r="K5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L5" t="s">
+        <v>91</v>
+      </c>
+      <c r="M5" t="s">
+        <v>26</v>
+      </c>
+      <c r="N5" t="s">
+        <v>96</v>
+      </c>
+      <c r="O5" t="s">
+        <v>27</v>
+      </c>
+      <c r="P5" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>28</v>
+      </c>
+      <c r="R5" t="s">
+        <v>104</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="T5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" t="s">
+        <v>74</v>
+      </c>
+      <c r="K6" t="s">
+        <v>32</v>
+      </c>
+      <c r="L6" t="s">
+        <v>92</v>
+      </c>
+      <c r="O6" t="s">
+        <v>33</v>
+      </c>
+      <c r="P6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" t="s">
+        <v>75</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="O7" t="s">
+        <v>37</v>
+      </c>
+      <c r="P7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" t="s">
-        <v>28</v>
-      </c>
-      <c r="I5" t="s">
-        <v>29</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="D9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9" t="s">
         <v>40</v>
       </c>
-      <c r="B9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="F9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" t="s">
         <v>42</v>
       </c>
-      <c r="C10" t="s">
+      <c r="F10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" t="s">
         <v>44</v>
       </c>
-      <c r="C11" t="s">
+      <c r="F11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" t="s">
         <v>46</v>
       </c>
-      <c r="C12" t="s">
+      <c r="F12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="D13" s="1"/>
+      <c r="E13" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
+      <c r="F13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="D14" s="1"/>
+      <c r="E14" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
+      <c r="F14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
+      <c r="F15" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="D16" s="1"/>
+      <c r="E16" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
-        <v>51</v>
+      <c r="F16" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="C1:S1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>